<commit_message>
hpc update some doc files about video6
</commit_message>
<xml_diff>
--- a/Ebbinghaus0524.xlsx
+++ b/Ebbinghaus0524.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="465" windowWidth="15945" windowHeight="12660" tabRatio="820"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="427">
   <si>
     <t>#5分钟</t>
   </si>
@@ -1320,13 +1320,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1、全局，以py为主 Ebbinghaus(py).xlsx
-2、Py_code下的运行时的error， py_errolog.txt
-3、Py_code下的code记录，6Python接口测试框架实战与自动化进阶.docx
-4、具体的code插入 来源，时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>议题</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1968,6 +1961,18 @@
     <t>检查字符串是否只包含十进制字符，如果是返回 true，否则返回 false。</t>
   </si>
   <si>
+    <t>Py\Py_code\practice\io和class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>django基础使用和原理特点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>requests基础使用和原理特点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>清理整合已有code，做到理解掌握，优先Py\Py_code\practice\.py</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1976,15 +1981,72 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Py\Py_code\practice\io和class</t>
+    <r>
+      <t xml:space="preserve">1、全局，以py为主 Ebbinghaus(py).xlsx
+2、Py_code下的运行时的error， py_errolog.txt
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3、Py_code下的code记录，6Python接口测试框架实战与自动化进阶.docx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4、具体的code插入 来源，时间</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据6视频和入门实践书</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据6视频和网络</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>django的接口开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据6视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>还是根据6往下走，遇到问题自己网上学一些相关知识</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2182,6 +2244,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -2320,7 +2390,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2542,6 +2612,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2732,7 +2805,7 @@
         <xdr:cNvPr id="2" name="图片 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2762,7 +2835,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2804,7 +2877,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2836,10 +2909,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2871,7 +2943,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3047,18 +3118,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="10.5" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="3"/>
@@ -3069,7 +3140,7 @@
         <v>224</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>223</v>
@@ -3086,21 +3157,21 @@
         <v>43607</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="23">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="49" customFormat="1">
+      <c r="A3" s="41">
         <v>43608</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="D3" s="23">
+      <c r="B3" s="30" t="s">
+        <v>419</v>
+      </c>
+      <c r="D3" s="76">
         <v>43609</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>418</v>
+      <c r="E3" s="49" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3108,7 +3179,39 @@
         <v>43609</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="23">
+        <v>43612</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="3" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -3120,7 +3223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -3140,27 +3243,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="C1" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="D1" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="E1" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="E1" s="59" t="s">
-        <v>232</v>
-      </c>
       <c r="F1" s="59" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="27">
       <c r="A2" s="60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B2" s="60" t="s">
         <v>99</v>
@@ -3207,10 +3310,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="61" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C7" s="61"/>
       <c r="D7" s="61"/>
@@ -3219,21 +3322,21 @@
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="60" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="60" t="s">
         <v>235</v>
-      </c>
-      <c r="C8" s="60" t="s">
-        <v>237</v>
-      </c>
-      <c r="D8" s="60" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="61" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C9" s="61"/>
       <c r="D9" s="61" t="s">
@@ -3241,26 +3344,26 @@
       </c>
       <c r="E9" s="61"/>
       <c r="F9" s="61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="60" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" s="60" t="s">
         <v>243</v>
       </c>
-      <c r="B10" s="60" t="s">
-        <v>242</v>
-      </c>
-      <c r="D10" s="60" t="s">
+      <c r="F10" s="60" t="s">
         <v>244</v>
-      </c>
-      <c r="F10" s="60" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="27">
       <c r="A11" s="61" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B11" s="61" t="s">
         <v>152</v>
@@ -3274,19 +3377,19 @@
     </row>
     <row r="12" spans="1:6" ht="40.5">
       <c r="A12" s="60" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B12" s="60" t="s">
         <v>153</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>154</v>
       </c>
       <c r="F12" s="60" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3317,10 +3420,10 @@
     </row>
     <row r="16" spans="1:6" ht="40.5">
       <c r="A16" s="60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B16" s="60" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C16" s="60" t="s">
         <v>123</v>
@@ -3343,7 +3446,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18" s="60" t="s">
         <v>159</v>
@@ -3360,7 +3463,7 @@
     </row>
     <row r="19" spans="1:6" ht="40.5">
       <c r="A19" s="61" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B19" s="61" t="s">
         <v>161</v>
@@ -4154,7 +4257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
@@ -4170,677 +4273,677 @@
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" thickBot="1">
       <c r="A1" s="62" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="B1" s="62" t="s">
-        <v>255</v>
-      </c>
       <c r="C1" s="62" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" thickBot="1">
       <c r="A2" s="75" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="66" t="s">
         <v>256</v>
       </c>
-      <c r="B2" s="66" t="s">
-        <v>257</v>
-      </c>
       <c r="C2" s="69" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" thickBot="1">
       <c r="A3" s="75" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="68" t="s">
         <v>258</v>
       </c>
-      <c r="B3" s="68" t="s">
-        <v>259</v>
-      </c>
       <c r="C3" s="71" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="26.25" thickBot="1">
       <c r="A4" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="B4" s="66" t="s">
         <v>260</v>
       </c>
-      <c r="B4" s="66" t="s">
-        <v>261</v>
-      </c>
       <c r="C4" s="72" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="27.75" thickBot="1">
       <c r="A5" s="75" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5" s="68" t="s">
         <v>262</v>
       </c>
-      <c r="B5" s="68" t="s">
-        <v>263</v>
-      </c>
       <c r="C5" s="64" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="27.75" thickBot="1">
       <c r="A6" s="75" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="66" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="66" t="s">
-        <v>265</v>
-      </c>
       <c r="C6" s="69" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="26.25" thickBot="1">
       <c r="A7" s="75" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7" s="68" t="s">
         <v>266</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>267</v>
-      </c>
       <c r="C7" s="63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="27.75" thickBot="1">
       <c r="A8" s="75" t="s">
+        <v>267</v>
+      </c>
+      <c r="B8" s="66" t="s">
         <v>268</v>
       </c>
-      <c r="B8" s="66" t="s">
-        <v>269</v>
-      </c>
       <c r="C8" s="72" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="39" thickBot="1">
       <c r="A9" s="75" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="68" t="s">
         <v>270</v>
       </c>
-      <c r="B9" s="68" t="s">
-        <v>271</v>
-      </c>
       <c r="C9" s="64" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" thickBot="1">
       <c r="A10" s="65" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10" s="66" t="s">
         <v>272</v>
       </c>
-      <c r="B10" s="66" t="s">
-        <v>273</v>
-      </c>
       <c r="C10" s="69" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="39" thickBot="1">
       <c r="A11" s="75" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" s="68" t="s">
         <v>274</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="C11" s="63" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="77" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="B12" s="70" t="s">
+        <v>276</v>
+      </c>
+      <c r="C12" s="72" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="76" t="s">
-        <v>276</v>
-      </c>
-      <c r="B12" s="70" t="s">
+    <row r="13" spans="1:3" ht="39" thickBot="1">
+      <c r="A13" s="78"/>
+      <c r="B13" s="71" t="s">
         <v>277</v>
       </c>
-      <c r="C12" s="72" t="s">
+      <c r="C13" s="74" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="77" t="s">
+        <v>278</v>
+      </c>
+      <c r="B14" s="73" t="s">
+        <v>279</v>
+      </c>
+      <c r="C14" s="69" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="39" thickBot="1">
-      <c r="A13" s="77"/>
-      <c r="B13" s="71" t="s">
-        <v>278</v>
-      </c>
-      <c r="C13" s="74" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="76" t="s">
-        <v>279</v>
-      </c>
-      <c r="B14" s="73" t="s">
+    <row r="15" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A15" s="78"/>
+      <c r="B15" s="74" t="s">
         <v>280</v>
       </c>
-      <c r="C14" s="69" t="s">
+      <c r="C15" s="63" t="s">
         <v>354</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A15" s="77"/>
-      <c r="B15" s="74" t="s">
-        <v>281</v>
-      </c>
-      <c r="C15" s="63" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" thickBot="1">
       <c r="A16" s="65" t="s">
+        <v>281</v>
+      </c>
+      <c r="B16" s="66" t="s">
         <v>282</v>
       </c>
-      <c r="B16" s="66" t="s">
-        <v>283</v>
-      </c>
       <c r="C16" s="72" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="39" thickBot="1">
       <c r="A17" s="75" t="s">
+        <v>283</v>
+      </c>
+      <c r="B17" s="68" t="s">
         <v>284</v>
       </c>
-      <c r="B17" s="68" t="s">
-        <v>285</v>
-      </c>
       <c r="C17" s="64" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="26.25" thickBot="1">
       <c r="A18" s="75" t="s">
+        <v>285</v>
+      </c>
+      <c r="B18" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="B18" s="66" t="s">
-        <v>287</v>
-      </c>
       <c r="C18" s="69" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26.25" thickBot="1">
       <c r="A19" s="75" t="s">
+        <v>287</v>
+      </c>
+      <c r="B19" s="68" t="s">
         <v>288</v>
       </c>
-      <c r="B19" s="68" t="s">
-        <v>289</v>
-      </c>
       <c r="C19" s="63" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" thickBot="1">
       <c r="A20" s="75" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" s="66" t="s">
         <v>290</v>
       </c>
-      <c r="B20" s="66" t="s">
-        <v>291</v>
-      </c>
       <c r="C20" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" thickBot="1">
       <c r="A21" s="75" t="s">
+        <v>291</v>
+      </c>
+      <c r="B21" s="68" t="s">
         <v>292</v>
       </c>
-      <c r="B21" s="68" t="s">
-        <v>293</v>
-      </c>
       <c r="C21" s="64" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="26.25" thickBot="1">
       <c r="A22" s="75" t="s">
+        <v>293</v>
+      </c>
+      <c r="B22" s="66" t="s">
         <v>294</v>
       </c>
-      <c r="B22" s="66" t="s">
-        <v>295</v>
-      </c>
       <c r="C22" s="69" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" thickBot="1">
       <c r="A23" s="75" t="s">
+        <v>295</v>
+      </c>
+      <c r="B23" s="68" t="s">
         <v>296</v>
       </c>
-      <c r="B23" s="68" t="s">
-        <v>297</v>
-      </c>
       <c r="C23" s="63" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" thickBot="1">
       <c r="A24" s="65" t="s">
+        <v>297</v>
+      </c>
+      <c r="B24" s="66" t="s">
         <v>298</v>
       </c>
-      <c r="B24" s="66" t="s">
-        <v>299</v>
-      </c>
       <c r="C24" s="72" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" thickBot="1">
       <c r="A25" s="67" t="s">
+        <v>299</v>
+      </c>
+      <c r="B25" s="68" t="s">
         <v>300</v>
       </c>
-      <c r="B25" s="68" t="s">
-        <v>301</v>
-      </c>
       <c r="C25" s="64" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" thickBot="1">
       <c r="A26" s="65" t="s">
+        <v>301</v>
+      </c>
+      <c r="B26" s="66" t="s">
         <v>302</v>
       </c>
-      <c r="B26" s="66" t="s">
-        <v>303</v>
-      </c>
       <c r="C26" s="69" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="39" thickBot="1">
       <c r="A27" s="67" t="s">
+        <v>303</v>
+      </c>
+      <c r="B27" s="68" t="s">
         <v>304</v>
       </c>
-      <c r="B27" s="68" t="s">
-        <v>305</v>
-      </c>
       <c r="C27" s="63" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" thickBot="1">
       <c r="A28" s="65" t="s">
+        <v>305</v>
+      </c>
+      <c r="B28" s="66" t="s">
         <v>306</v>
       </c>
-      <c r="B28" s="66" t="s">
-        <v>307</v>
-      </c>
       <c r="C28" s="72" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="26.25" thickBot="1">
       <c r="A29" s="67" t="s">
+        <v>307</v>
+      </c>
+      <c r="B29" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="B29" s="68" t="s">
-        <v>309</v>
-      </c>
       <c r="C29" s="64" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="51.75" thickBot="1">
       <c r="A30" s="65" t="s">
+        <v>309</v>
+      </c>
+      <c r="B30" s="66" t="s">
         <v>310</v>
       </c>
-      <c r="B30" s="66" t="s">
-        <v>311</v>
-      </c>
       <c r="C30" s="69" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="27.75" thickBot="1">
       <c r="A31" s="67" t="s">
+        <v>311</v>
+      </c>
+      <c r="B31" s="68" t="s">
         <v>312</v>
       </c>
-      <c r="B31" s="68" t="s">
-        <v>313</v>
-      </c>
       <c r="C31" s="63" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" thickBot="1">
       <c r="A32" s="65" t="s">
+        <v>313</v>
+      </c>
+      <c r="B32" s="66" t="s">
         <v>314</v>
       </c>
-      <c r="B32" s="66" t="s">
-        <v>315</v>
-      </c>
       <c r="C32" s="72" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26.25" thickBot="1">
       <c r="A33" s="67" t="s">
+        <v>315</v>
+      </c>
+      <c r="B33" s="68" t="s">
         <v>316</v>
       </c>
-      <c r="B33" s="68" t="s">
-        <v>317</v>
-      </c>
       <c r="C33" s="64" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" thickBot="1">
       <c r="A34" s="65" t="s">
+        <v>317</v>
+      </c>
+      <c r="B34" s="66" t="s">
         <v>318</v>
       </c>
-      <c r="B34" s="66" t="s">
-        <v>319</v>
-      </c>
       <c r="C34" s="69" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="39" thickBot="1">
       <c r="A35" s="67" t="s">
+        <v>319</v>
+      </c>
+      <c r="B35" s="68" t="s">
         <v>320</v>
       </c>
-      <c r="B35" s="68" t="s">
-        <v>321</v>
-      </c>
       <c r="C35" s="63" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" thickBot="1">
       <c r="A36" s="65" t="s">
+        <v>321</v>
+      </c>
+      <c r="B36" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="B36" s="66" t="s">
-        <v>323</v>
-      </c>
       <c r="C36" s="72" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="26.25" thickBot="1">
       <c r="A37" s="67" t="s">
+        <v>323</v>
+      </c>
+      <c r="B37" s="68" t="s">
         <v>324</v>
       </c>
-      <c r="B37" s="68" t="s">
-        <v>325</v>
-      </c>
       <c r="C37" s="64" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="39" thickBot="1">
       <c r="A38" s="65" t="s">
+        <v>325</v>
+      </c>
+      <c r="B38" s="66" t="s">
         <v>326</v>
       </c>
-      <c r="B38" s="66" t="s">
-        <v>327</v>
-      </c>
       <c r="C38" s="69" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="26.25" thickBot="1">
       <c r="A39" s="67" t="s">
+        <v>327</v>
+      </c>
+      <c r="B39" s="68" t="s">
         <v>328</v>
       </c>
-      <c r="B39" s="68" t="s">
-        <v>329</v>
-      </c>
       <c r="C39" s="63" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" thickBot="1">
       <c r="A40" s="65" t="s">
+        <v>329</v>
+      </c>
+      <c r="B40" s="66" t="s">
         <v>330</v>
       </c>
-      <c r="B40" s="66" t="s">
-        <v>331</v>
-      </c>
       <c r="C40" s="72" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="26.25" thickBot="1">
       <c r="A41" s="67" t="s">
+        <v>331</v>
+      </c>
+      <c r="B41" s="68" t="s">
         <v>332</v>
       </c>
-      <c r="B41" s="68" t="s">
-        <v>333</v>
-      </c>
       <c r="C41" s="64" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="26.25" thickBot="1">
       <c r="A42" s="65" t="s">
+        <v>333</v>
+      </c>
+      <c r="B42" s="66" t="s">
         <v>334</v>
       </c>
-      <c r="B42" s="66" t="s">
+      <c r="C42" s="69" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" thickBot="1">
+      <c r="A43" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="C42" s="69" t="s">
+      <c r="B43" s="73" t="s">
+        <v>336</v>
+      </c>
+      <c r="C43" s="63" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.25" thickBot="1">
-      <c r="A43" s="78" t="s">
-        <v>336</v>
-      </c>
-      <c r="B43" s="73" t="s">
+    <row r="44" spans="1:3" ht="14.25" thickBot="1">
+      <c r="A44" s="80"/>
+      <c r="B44" s="74" t="s">
         <v>337</v>
       </c>
-      <c r="C43" s="63" t="s">
+      <c r="C44" s="72" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" thickBot="1">
-      <c r="A44" s="79"/>
-      <c r="B44" s="74" t="s">
-        <v>338</v>
-      </c>
-      <c r="C44" s="72" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" thickBot="1">
       <c r="A45" s="65" t="s">
+        <v>338</v>
+      </c>
+      <c r="B45" s="66" t="s">
         <v>339</v>
       </c>
-      <c r="B45" s="66" t="s">
-        <v>340</v>
-      </c>
       <c r="C45" s="64" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" thickBot="1">
       <c r="A46" s="67" t="s">
+        <v>340</v>
+      </c>
+      <c r="B46" s="68" t="s">
         <v>341</v>
       </c>
-      <c r="B46" s="68" t="s">
-        <v>342</v>
-      </c>
       <c r="C46" s="69" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="39" thickBot="1">
       <c r="C47" s="63" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="C48" s="72" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" spans="3:3" ht="14.25" thickBot="1">
       <c r="C49" s="64" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" s="69" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="51" spans="3:3" ht="14.25" thickBot="1">
       <c r="C51" s="63" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52" s="72" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="53" spans="3:3" ht="26.25" thickBot="1">
       <c r="C53" s="64" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="54" spans="3:3">
       <c r="C54" s="69" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="55" spans="3:3" ht="14.25" thickBot="1">
       <c r="C55" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="56" spans="3:3">
       <c r="C56" s="72" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="57" spans="3:3" ht="14.25" thickBot="1">
       <c r="C57" s="64" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="3:3">
       <c r="C58" s="69" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="59" spans="3:3" ht="26.25" thickBot="1">
       <c r="C59" s="63" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="60" spans="3:3">
       <c r="C60" s="72" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="61" spans="3:3" ht="14.25" thickBot="1">
       <c r="C61" s="64" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="3:3">
       <c r="C62" s="69" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="63" spans="3:3" ht="26.25" thickBot="1">
       <c r="C63" s="63" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="64" spans="3:3">
       <c r="C64" s="72" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="65" spans="3:3" ht="39" thickBot="1">
       <c r="C65" s="64" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" s="69" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="67" spans="3:3" ht="39" thickBot="1">
       <c r="C67" s="63" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="68" spans="3:3">
       <c r="C68" s="72" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="69" spans="3:3" ht="14.25" thickBot="1">
       <c r="C69" s="64" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="70" spans="3:3">
       <c r="C70" s="69" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="71" spans="3:3" ht="14.25" thickBot="1">
       <c r="C71" s="63" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="72" spans="3:3">
       <c r="C72" s="72" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="73" spans="3:3" ht="26.25" thickBot="1">
       <c r="C73" s="64" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="74" spans="3:3">
       <c r="C74" s="69" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="75" spans="3:3" ht="26.25" thickBot="1">
       <c r="C75" s="63" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="76" spans="3:3">
       <c r="C76" s="72" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="77" spans="3:3" ht="14.25" thickBot="1">
       <c r="C77" s="64" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="78" spans="3:3">
       <c r="C78" s="69" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="79" spans="3:3" ht="14.25" thickBot="1">
       <c r="C79" s="63" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="80" spans="3:3">
       <c r="C80" s="72" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="81" spans="3:3" ht="26.25" thickBot="1">
       <c r="C81" s="64" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -4939,7 +5042,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5017,7 +5120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5259,7 +5362,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -5540,7 +5643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5679,7 +5782,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5896,7 +5999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5935,7 +6038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E83"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">

</xml_diff>